<commit_message>
All features are now ready and useable. Groups are craeted in the create_validation_clients.py file and only 1 feature per group is selected.
</commit_message>
<xml_diff>
--- a/validation_excel.xlsx
+++ b/validation_excel.xlsx
@@ -7,22 +7,22 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="drgqybcoei" sheetId="1" r:id="rId1"/>
-    <sheet name="vzsjfkabit" sheetId="2" r:id="rId2"/>
-    <sheet name="uljcqzbgfo" sheetId="3" r:id="rId3"/>
-    <sheet name="lswdazrkcf" sheetId="4" r:id="rId4"/>
-    <sheet name="fwdrkvuham" sheetId="5" r:id="rId5"/>
-    <sheet name="ifvtpwrsqm" sheetId="6" r:id="rId6"/>
-    <sheet name="vnhzfmtkqe" sheetId="7" r:id="rId7"/>
-    <sheet name="zlvndycprt" sheetId="8" r:id="rId8"/>
-    <sheet name="zuqixbypom" sheetId="9" r:id="rId9"/>
+    <sheet name="jcfkzlaygq" sheetId="1" r:id="rId1"/>
+    <sheet name="jfcdbzxwyg" sheetId="2" r:id="rId2"/>
+    <sheet name="awfmohbzds" sheetId="3" r:id="rId3"/>
+    <sheet name="imkeztnpwo" sheetId="4" r:id="rId4"/>
+    <sheet name="njiptxqrco" sheetId="5" r:id="rId5"/>
+    <sheet name="pofhjriasl" sheetId="6" r:id="rId6"/>
+    <sheet name="lpbaxngedz" sheetId="7" r:id="rId7"/>
+    <sheet name="ydwiotbnle" sheetId="8" r:id="rId8"/>
+    <sheet name="iwjaochfeq" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="151">
   <si>
     <t>translationSetId</t>
   </si>
@@ -30,292 +30,451 @@
     <t>museumname</t>
   </si>
   <si>
+    <t>gardens</t>
+  </si>
+  <si>
+    <t>cluster0</t>
+  </si>
+  <si>
+    <t>weelchair</t>
+  </si>
+  <si>
+    <t>museum total</t>
+  </si>
+  <si>
+    <t>feature total</t>
+  </si>
+  <si>
+    <t>1335f2de-05b0-4351-8cae-1cb1263b3791</t>
+  </si>
+  <si>
+    <t>0d9b11c5-4842-4d97-b105-908bca7c8fa5</t>
+  </si>
+  <si>
+    <t>9dd3fd7c-9281-4e0b-a661-909e597b93ee</t>
+  </si>
+  <si>
+    <t>8fae9e9b-5c62-477b-9ccc-d9d3ec1d695c</t>
+  </si>
+  <si>
+    <t>971a3945-faba-4021-8d5b-5b6fcd124640</t>
+  </si>
+  <si>
+    <t>c5f783ea-db8b-4a9b-93bb-311d51687719</t>
+  </si>
+  <si>
+    <t>c7858635-11bf-473d-9dc7-7336bbbd29ca</t>
+  </si>
+  <si>
+    <t>d9c3694b-8999-46e7-9264-66e2ca190c86</t>
+  </si>
+  <si>
+    <t>93062e20-901e-46a2-b1f4-107cd82e7ed5</t>
+  </si>
+  <si>
+    <t>c4cc477e-1442-4ef9-96ea-539e46356b07</t>
+  </si>
+  <si>
+    <t>Het Scheepvaartmuseum</t>
+  </si>
+  <si>
+    <t>Museum Speelklok</t>
+  </si>
+  <si>
+    <t>Museum Rotterdam</t>
+  </si>
+  <si>
+    <t>Nederlands Zilvermuseum</t>
+  </si>
+  <si>
+    <t>Zuiderzeemuseum</t>
+  </si>
+  <si>
+    <t>Het Utrechts Archief</t>
+  </si>
+  <si>
+    <t>Maritiem Museum Rotterdam</t>
+  </si>
+  <si>
+    <t>Veiligheidsmuseum PIT</t>
+  </si>
+  <si>
+    <t>Nationaal Tinnen Figuren Museum</t>
+  </si>
+  <si>
+    <t>Louis Couperus Museum</t>
+  </si>
+  <si>
+    <t>cluster5</t>
+  </si>
+  <si>
+    <t>cluster8</t>
+  </si>
+  <si>
+    <t>92652b8f-7600-4bee-8640-1c40b21a32cf</t>
+  </si>
+  <si>
+    <t>aa8279d3-78cf-4af8-8f83-24dd44caabd6</t>
+  </si>
+  <si>
+    <t>d579493e-5364-4327-b712-d231508db640</t>
+  </si>
+  <si>
+    <t>7a6bb20e-440e-428d-a735-e417b43aa8a9</t>
+  </si>
+  <si>
+    <t>64669da3-83b4-421d-a306-4f0c6669d7db</t>
+  </si>
+  <si>
+    <t>630f0ad9-d790-4a77-a847-e7acb31be6d8</t>
+  </si>
+  <si>
+    <t>e16ae770-865f-47d5-99ff-6ae6fc094217</t>
+  </si>
+  <si>
+    <t>addebae4-6756-4fe4-b59c-1aac2d80ab8e</t>
+  </si>
+  <si>
+    <t>1f85673a-ba18-4aaf-821a-baf56c7efea7</t>
+  </si>
+  <si>
+    <t>a8d715f7-82f5-4df4-9308-0d33c4c1eaa2</t>
+  </si>
+  <si>
+    <t>Museum Van Loon</t>
+  </si>
+  <si>
+    <t>Amsterdam Museum</t>
+  </si>
+  <si>
+    <t>Portrait Gallery of the 17th Century</t>
+  </si>
+  <si>
+    <t>Museum Willet-Holthuysen</t>
+  </si>
+  <si>
+    <t>Grachtenmuseum Amsterdam</t>
+  </si>
+  <si>
+    <t>De Hollandsche Manege</t>
+  </si>
+  <si>
+    <t>Weegschaal Museum Naarden</t>
+  </si>
+  <si>
+    <t>Museum Paulina Bisdom van Vliet</t>
+  </si>
+  <si>
+    <t>Hermitage Amsterdam</t>
+  </si>
+  <si>
+    <t>Koninklijk Paleis Amsterdam</t>
+  </si>
+  <si>
+    <t>cluster7</t>
+  </si>
+  <si>
+    <t>1a918684-33d5-485a-80b7-90a8086803ef</t>
+  </si>
+  <si>
+    <t>56518036-a7ca-43fe-b010-2ddfcec6aca3</t>
+  </si>
+  <si>
+    <t>5ebaa739-b1a4-443b-9cde-6c0b18e81607</t>
+  </si>
+  <si>
+    <t>053014de-f18f-45e3-8dc6-c3f907646311</t>
+  </si>
+  <si>
+    <t>b95305d9-cc57-498c-8819-c1983713d181</t>
+  </si>
+  <si>
+    <t>10f92ca9-be97-40d2-b2ad-cb99d5154981</t>
+  </si>
+  <si>
+    <t>078fe561-4a1d-4712-b204-11913bdd57b4</t>
+  </si>
+  <si>
+    <t>e9ad0209-89ad-4e53-a353-b7328562f8e6</t>
+  </si>
+  <si>
+    <t>fb5c119f-f4a1-411c-a943-f609fcb5f5f3</t>
+  </si>
+  <si>
+    <t>f9d5d350-4bab-499a-8f53-2af1f6f25601</t>
+  </si>
+  <si>
+    <t>Buitenplaats Kasteel Wijlre</t>
+  </si>
+  <si>
+    <t>Mauritshuis</t>
+  </si>
+  <si>
+    <t>Museon</t>
+  </si>
+  <si>
+    <t>Museum De Domijnen, afdeling Hedendaagse Kunst</t>
+  </si>
+  <si>
+    <t>Keramiekcentrum Tiendschuur Tegelen</t>
+  </si>
+  <si>
+    <t>Marres, Huis voor Hedendaagse Kunst</t>
+  </si>
+  <si>
+    <t>Kunstvereniging Diepenheim</t>
+  </si>
+  <si>
+    <t>Universiteitsmuseum Groningen</t>
+  </si>
+  <si>
+    <t>Museum Swaensteyn</t>
+  </si>
+  <si>
+    <t>Trompenburg Tuinen &amp; Arboretum</t>
+  </si>
+  <si>
+    <t>lecture</t>
+  </si>
+  <si>
+    <t>educative</t>
+  </si>
+  <si>
+    <t>1d9c7610-ab17-4f68-ae48-9cefefc32b20</t>
+  </si>
+  <si>
+    <t>3caa2392-510f-4c85-a489-b83e8200ff90</t>
+  </si>
+  <si>
+    <t>9231914a-1dac-4afe-b28a-cc37ee7c5bfd</t>
+  </si>
+  <si>
+    <t>ddc06b8b-9dd1-4768-be15-75477b0f104a</t>
+  </si>
+  <si>
+    <t>27b9e34f-c9da-47d5-a22e-d5140b9b0d18</t>
+  </si>
+  <si>
+    <t>a42cba4d-03ab-449a-8fb5-a24fb363afa5</t>
+  </si>
+  <si>
+    <t>1cf7d97e-57d6-4550-be98-8d19ea5ac3a5</t>
+  </si>
+  <si>
+    <t>Continium discovery center</t>
+  </si>
+  <si>
+    <t>Luchtvaartmuseum Aviodrome</t>
+  </si>
+  <si>
+    <t>Streek &amp; Landbouwmuseum Goemanszorg</t>
+  </si>
+  <si>
+    <t>Spoorwegmuseum</t>
+  </si>
+  <si>
+    <t>Museum Sterrenwacht Sonnenborgh</t>
+  </si>
+  <si>
+    <t>Belasting &amp; Douane Museum</t>
+  </si>
+  <si>
+    <t>Pieter Vermeulen Museum</t>
+  </si>
+  <si>
+    <t>cluster6</t>
+  </si>
+  <si>
+    <t>openair</t>
+  </si>
+  <si>
+    <t>visual</t>
+  </si>
+  <si>
+    <t>b5d597b1-730f-402b-bc6e-a86cadebd973</t>
+  </si>
+  <si>
+    <t>f57a988c-883e-4f75-8dc6-7d5f76d005e5</t>
+  </si>
+  <si>
+    <t>673dafbb-e461-4ffb-ab3c-f857358c77a7</t>
+  </si>
+  <si>
+    <t>15521a24-f0fd-49c2-beef-dcfcca62e2e7</t>
+  </si>
+  <si>
+    <t>38a216ca-1fee-45de-9b0a-ae857342d0c0</t>
+  </si>
+  <si>
+    <t>d393d962-7ee9-411b-8c60-c0879d6e3fd7</t>
+  </si>
+  <si>
+    <t>944a4c15-58c0-44dc-8f8a-c65b44179c16</t>
+  </si>
+  <si>
+    <t>Geologisch Museum Hofland</t>
+  </si>
+  <si>
+    <t>Museum Terra Maris</t>
+  </si>
+  <si>
+    <t>Cube Design Museum</t>
+  </si>
+  <si>
+    <t>De Kuiperij</t>
+  </si>
+  <si>
+    <t>Botanische Tuin TU Delft</t>
+  </si>
+  <si>
+    <t>Micropia</t>
+  </si>
+  <si>
+    <t>Missiemuseum Steyl</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>cc12b367-a374-4c8a-bd04-8b24e412af3c</t>
+  </si>
+  <si>
+    <t>b0654f59-55d5-4c74-8420-3d3938f861e2</t>
+  </si>
+  <si>
+    <t>9c4bddf8-9bef-46cb-a2ef-5f13ba85884f</t>
+  </si>
+  <si>
+    <t>f7e3d4b2-ae53-41c5-aa79-cfa323796de7</t>
+  </si>
+  <si>
+    <t>044424ba-e4e7-4de8-b88c-ccaf14cf4c59</t>
+  </si>
+  <si>
+    <t>1de93dee-f6b5-4a1c-8d7f-e896df26a694</t>
+  </si>
+  <si>
+    <t>7433df02-7eee-40bc-a5c5-98fb3373fbc9</t>
+  </si>
+  <si>
+    <t>Nederlands Openluchtmuseum</t>
+  </si>
+  <si>
+    <t>Botanische Tuin De Kruidhof</t>
+  </si>
+  <si>
+    <t>Nederlands Watermuseum</t>
+  </si>
+  <si>
+    <t>Paviljoen Nederland en WOI</t>
+  </si>
+  <si>
+    <t>Honig Breethuis</t>
+  </si>
+  <si>
+    <t>Literatuurmuseum</t>
+  </si>
+  <si>
+    <t>Museum Tot Zover</t>
+  </si>
+  <si>
+    <t>cluster2</t>
+  </si>
+  <si>
     <t>culture</t>
   </si>
   <si>
-    <t>history</t>
-  </si>
-  <si>
-    <t>tech</t>
-  </si>
-  <si>
-    <t>museum total</t>
-  </si>
-  <si>
-    <t>feature total</t>
-  </si>
-  <si>
-    <t>944a4c15-58c0-44dc-8f8a-c65b44179c16</t>
-  </si>
-  <si>
-    <t>38a216ca-1fee-45de-9b0a-ae857342d0c0</t>
-  </si>
-  <si>
-    <t>b5d597b1-730f-402b-bc6e-a86cadebd973</t>
-  </si>
-  <si>
-    <t>f57a988c-883e-4f75-8dc6-7d5f76d005e5</t>
-  </si>
-  <si>
-    <t>5ebaa739-b1a4-443b-9cde-6c0b18e81607</t>
-  </si>
-  <si>
-    <t>d393d962-7ee9-411b-8c60-c0879d6e3fd7</t>
-  </si>
-  <si>
-    <t>e9ad0209-89ad-4e53-a353-b7328562f8e6</t>
-  </si>
-  <si>
-    <t>f42e58c1-d6e6-4bdb-aa51-e0af569e31df</t>
-  </si>
-  <si>
-    <t>1cf7d97e-57d6-4550-be98-8d19ea5ac3a5</t>
-  </si>
-  <si>
-    <t>f82c9249-ae42-4690-bcbc-9db3f55db2d0</t>
-  </si>
-  <si>
-    <t>Missiemuseum Steyl</t>
-  </si>
-  <si>
-    <t>Botanische Tuin TU Delft</t>
-  </si>
-  <si>
-    <t>Geologisch Museum Hofland</t>
-  </si>
-  <si>
-    <t>Museum Terra Maris</t>
-  </si>
-  <si>
-    <t>Museon</t>
-  </si>
-  <si>
-    <t>Micropia</t>
-  </si>
-  <si>
-    <t>Universiteitsmuseum Groningen</t>
-  </si>
-  <si>
-    <t>Joods Historisch Museum</t>
-  </si>
-  <si>
-    <t>Pieter Vermeulen Museum</t>
-  </si>
-  <si>
-    <t>Natuurmuseum Fryslân</t>
-  </si>
-  <si>
-    <t>openair</t>
-  </si>
-  <si>
-    <t>library</t>
-  </si>
-  <si>
     <t>832cd1d6-c933-4279-8ae6-1e3fa38853a2</t>
   </si>
   <si>
+    <t>a6fc14aa-84ee-4c59-8801-baf29c2557dd</t>
+  </si>
+  <si>
+    <t>cda45f48-2deb-4062-bd6f-ad4da92c8114</t>
+  </si>
+  <si>
+    <t>fbd0f6e4-105e-4b04-bf93-9b06a40e7204</t>
+  </si>
+  <si>
+    <t>424e8423-e43b-48e8-ad19-821014020860</t>
+  </si>
+  <si>
+    <t>Museum de Kantfabriek</t>
+  </si>
+  <si>
+    <t>Museum Huis Doorn</t>
+  </si>
+  <si>
+    <t>Museummolen en molenwinkel De Walvisch</t>
+  </si>
+  <si>
+    <t>Historisch Museum Haarlemmermeer</t>
+  </si>
+  <si>
+    <t>Comenius Museum</t>
+  </si>
+  <si>
+    <t>fde0ab33-2d85-4f29-a0fb-6e13a6f52142</t>
+  </si>
+  <si>
+    <t>3b0519ec-a69a-4f2f-8ea2-a5ac4428d096</t>
+  </si>
+  <si>
+    <t>39c0d207-7edc-4e51-82bb-e0d0da3576d4</t>
+  </si>
+  <si>
+    <t>368607b3-1085-4b46-9f41-3204431b0545</t>
+  </si>
+  <si>
+    <t>Het Nieuwe Instituut</t>
+  </si>
+  <si>
+    <t>Nederlands Fotomuseum</t>
+  </si>
+  <si>
+    <t>Stadhuismuseum Zierikzee</t>
+  </si>
+  <si>
+    <t>Historiehuis Roermond</t>
+  </si>
+  <si>
+    <t>science</t>
+  </si>
+  <si>
+    <t>a2040f47-849b-4ca6-967e-adee1ee5a930</t>
+  </si>
+  <si>
+    <t>682197a8-0359-4094-8281-ffa059de480f</t>
+  </si>
+  <si>
+    <t>798b12be-0127-4f41-91df-1a5e71af1e37</t>
+  </si>
+  <si>
     <t>7810d0eb-0034-457b-9cf7-ae7aa21e104f</t>
   </si>
   <si>
-    <t>044424ba-e4e7-4de8-b88c-ccaf14cf4c59</t>
-  </si>
-  <si>
-    <t>23eaf7fc-a6ca-40a3-87c5-257dca174595</t>
-  </si>
-  <si>
-    <t>424e8423-e43b-48e8-ad19-821014020860</t>
+    <t>95a74653-495e-4420-82e0-a1a6195f974d</t>
   </si>
   <si>
     <t>6add9957-7a8c-469f-83da-ff169b0f2050</t>
   </si>
   <si>
-    <t>a8d715f7-82f5-4df4-9308-0d33c4c1eaa2</t>
-  </si>
-  <si>
-    <t>c5ad38ca-1303-43d2-adee-04bb0e3268f6</t>
-  </si>
-  <si>
-    <t>Museum de Kantfabriek</t>
+    <t>TextielMuseum</t>
+  </si>
+  <si>
+    <t>Museum Catharijneconvent</t>
+  </si>
+  <si>
+    <t>De Looierij</t>
   </si>
   <si>
     <t>Rijksmuseum Amsterdam</t>
   </si>
   <si>
-    <t>Honig Breethuis</t>
-  </si>
-  <si>
-    <t>Nationaal Onderduikmuseum</t>
-  </si>
-  <si>
-    <t>Comenius Museum</t>
+    <t>Museum De Lakenhal</t>
   </si>
   <si>
     <t>Louwman Museum</t>
-  </si>
-  <si>
-    <t>Koninklijk Paleis Amsterdam</t>
-  </si>
-  <si>
-    <t>Stedelijk Museum Alkmaar</t>
-  </si>
-  <si>
-    <t>f05af616-d419-463e-89da-c107b2f20129</t>
-  </si>
-  <si>
-    <t>a42cba4d-03ab-449a-8fb5-a24fb363afa5</t>
-  </si>
-  <si>
-    <t>971a3945-faba-4021-8d5b-5b6fcd124640</t>
-  </si>
-  <si>
-    <t>Museum Het Valkhof</t>
-  </si>
-  <si>
-    <t>Belasting &amp; Douane Museum</t>
-  </si>
-  <si>
-    <t>Zuiderzeemuseum</t>
-  </si>
-  <si>
-    <t>550e313e-c3f0-406c-b4d3-01dbce024096</t>
-  </si>
-  <si>
-    <t>8f9a43db-d28a-4857-b4e5-2f128210a7ee</t>
-  </si>
-  <si>
-    <t>b9fa7554-70fd-4a40-8515-55ff3895e129</t>
-  </si>
-  <si>
-    <t>4f05881b-f742-480c-b13d-91d99c6fc4a2</t>
-  </si>
-  <si>
-    <t>Museum Collectie Brands</t>
-  </si>
-  <si>
-    <t>Museum 't Oude Slot</t>
-  </si>
-  <si>
-    <t>t Fiskershúske</t>
-  </si>
-  <si>
-    <t>Veenkoloniaal Museum</t>
-  </si>
-  <si>
-    <t>naval</t>
-  </si>
-  <si>
-    <t>d280a91d-ebc1-4607-afb9-e38a67c862d0</t>
-  </si>
-  <si>
-    <t>a2040f47-849b-4ca6-967e-adee1ee5a930</t>
-  </si>
-  <si>
-    <t>8fae9e9b-5c62-477b-9ccc-d9d3ec1d695c</t>
-  </si>
-  <si>
-    <t>dffe8ae8-e39f-49d2-a41b-004775a406a8</t>
-  </si>
-  <si>
-    <t>5ea552c8-0db1-4e75-b6b0-d5b5933a5f2f</t>
-  </si>
-  <si>
-    <t>Wereldmuseum Rotterdam</t>
-  </si>
-  <si>
-    <t>TextielMuseum</t>
-  </si>
-  <si>
-    <t>Nederlands Zilvermuseum</t>
-  </si>
-  <si>
-    <t>Portugese Synagoge Amsterdam</t>
-  </si>
-  <si>
-    <t>Limburgs Museum</t>
-  </si>
-  <si>
-    <t>d1e42c4d-d176-4833-98a8-a3fb4a725b91</t>
-  </si>
-  <si>
-    <t>e89e2757-e3e7-4d22-bba5-58f4164a0105</t>
-  </si>
-  <si>
-    <t>4b596778-4379-48da-a946-0d04e39e3cea</t>
-  </si>
-  <si>
-    <t>Museumpark Archeon</t>
-  </si>
-  <si>
-    <t>Museum Staphorst</t>
-  </si>
-  <si>
-    <t>Museum Het Pakhuis</t>
-  </si>
-  <si>
-    <t>621c0554-f8d1-454c-9218-e60683a536ee</t>
-  </si>
-  <si>
-    <t>1de93dee-f6b5-4a1c-8d7f-e896df26a694</t>
-  </si>
-  <si>
-    <t>mij | museum ijsselstein</t>
-  </si>
-  <si>
-    <t>Literatuurmuseum</t>
-  </si>
-  <si>
-    <t>1e3aaa11-c04f-43bd-9707-58401ee41056</t>
-  </si>
-  <si>
-    <t>b2398575-3c86-42a2-b07c-886384eb9add</t>
-  </si>
-  <si>
-    <t>682197a8-0359-4094-8281-ffa059de480f</t>
-  </si>
-  <si>
-    <t>Hunebedcentrum</t>
-  </si>
-  <si>
-    <t>Museum Wierdenland Ezinge</t>
-  </si>
-  <si>
-    <t>Museum Catharijneconvent</t>
-  </si>
-  <si>
-    <t>visual</t>
-  </si>
-  <si>
-    <t>ethnology</t>
-  </si>
-  <si>
-    <t>798b12be-0127-4f41-91df-1a5e71af1e37</t>
-  </si>
-  <si>
-    <t>e4b87fd4-b473-4137-abdc-c6854b3dd7a4</t>
-  </si>
-  <si>
-    <t>ddc06b8b-9dd1-4768-be15-75477b0f104a</t>
-  </si>
-  <si>
-    <t>3caa2392-510f-4c85-a489-b83e8200ff90</t>
-  </si>
-  <si>
-    <t>689733f3-0f0a-411d-b5b4-a33dd39639f0</t>
-  </si>
-  <si>
-    <t>De Looierij</t>
-  </si>
-  <si>
-    <t>Nederlands Artillerie Museum</t>
-  </si>
-  <si>
-    <t>Spoorwegmuseum</t>
-  </si>
-  <si>
-    <t>Luchtvaartmuseum Aviodrome</t>
-  </si>
-  <si>
-    <t>Museum Weesp</t>
   </si>
 </sst>
 </file>
@@ -701,7 +860,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>280</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -716,15 +875,15 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>110</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -739,15 +898,15 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>354</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -759,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -770,7 +929,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>471</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -785,15 +944,15 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>186</v>
+        <v>290</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -816,7 +975,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>419</v>
+        <v>387</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -839,7 +998,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>450</v>
+        <v>388</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -848,7 +1007,7 @@
         <v>23</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -857,12 +1016,12 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>468</v>
+        <v>430</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -871,13 +1030,13 @@
         <v>24</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -885,7 +1044,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>57</v>
+        <v>277</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -908,7 +1067,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>478</v>
+        <v>384</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -923,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -934,16 +1093,16 @@
         <v>6</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -981,22 +1140,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1004,13 +1163,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>450</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1027,16 +1186,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>230</v>
+        <v>423</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1045,27 +1204,27 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>9</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1073,16 +1232,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>468</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1091,41 +1250,41 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>133</v>
+        <v>443</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1142,22 +1301,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>208</v>
+        <v>340</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1165,13 +1324,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>328</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1180,33 +1339,33 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>386</v>
+        <v>328</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1217,13 +1376,13 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G12">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1233,13 +1392,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1247,38 +1406,44 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>230</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>468</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1286,152 +1451,182 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>359</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
         <v>450</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>462</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>386</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>316</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
-        <v>133</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1">
-        <v>75</v>
-      </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>250</v>
+        <v>488</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>290</v>
+        <v>483</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1441,13 +1636,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1455,154 +1650,262 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>430</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>272</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>436</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
         <v>316</v>
       </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>290</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>462</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>468</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>266</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>361</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
         <v>57</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>450</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>157</v>
-      </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>0</v>
       </c>
     </row>
@@ -1627,13 +1930,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1641,13 +1944,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>468</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1656,44 +1959,44 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>417</v>
+        <v>471</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1702,21 +2005,21 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>450</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1733,13 +2036,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>313</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1748,24 +2051,24 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1774,18 +2077,18 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>268</v>
+        <v>384</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1794,21 +2097,21 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>440</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1817,21 +2120,21 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>185</v>
+        <v>419</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1840,21 +2143,21 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1863,10 +2166,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1880,10 +2183,10 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1893,13 +2196,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1910,61 +2213,70 @@
         <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>250</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1975,16 +2287,19 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>75</v>
+        <v>344</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1995,79 +2310,91 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>448</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>468</v>
+        <v>301</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>450</v>
+        <v>476</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>114</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>133</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2075,16 +2402,19 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>145</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2095,16 +2425,19 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>386</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2115,19 +2448,25 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2151,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -2165,13 +2504,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>185</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2188,13 +2527,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>440</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2203,21 +2542,21 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2226,21 +2565,21 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>313</v>
+        <v>436</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2249,21 +2588,21 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>194</v>
+        <v>324</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2280,13 +2619,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>450</v>
+        <v>402</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2303,13 +2642,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>60</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2326,36 +2665,36 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>462</v>
+        <v>489</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>268</v>
+        <v>316</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2364,30 +2703,30 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -2398,16 +2737,16 @@
         <v>6</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G12">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2417,13 +2756,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2431,27 +2770,24 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>450</v>
+        <v>494</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2462,22 +2798,19 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>354</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2485,137 +2818,119 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>419</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>316</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>471</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1">
-        <v>186</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1">
-        <v>60</v>
-      </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>65</v>
+        <v>436</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2623,22 +2938,19 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>347</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2646,22 +2958,19 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>202</v>
+        <v>401</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2669,25 +2978,19 @@
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2711,10 +3014,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -2722,39 +3025,39 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>250</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2762,19 +3065,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2782,79 +3085,79 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>436</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>119</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>316</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2862,59 +3165,59 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>450</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -2925,13 +3228,13 @@
         <v>6</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>